<commit_message>
Modification to the network and scenario data  to make it more clear to the user
</commit_message>
<xml_diff>
--- a/Power_System/data/power_network.xlsx
+++ b/Power_System/data/power_network.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\Adam_Project\Powe_Generation_Distribution_and_Consumption\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\Apps\demos\Power_System\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,16 +15,14 @@
     <sheet name="network" sheetId="3" r:id="rId1"/>
     <sheet name="nodes" sheetId="4" r:id="rId2"/>
     <sheet name="links" sheetId="8" r:id="rId3"/>
-    <sheet name="groups" sheetId="10" r:id="rId4"/>
-    <sheet name="groups_members" sheetId="11" r:id="rId5"/>
-    <sheet name="attributes" sheetId="2" r:id="rId6"/>
-    <sheet name="rules" sheetId="13" r:id="rId7"/>
-    <sheet name="connectivity_matrix" sheetId="12" r:id="rId8"/>
-    <sheet name="fixed_power_flow" sheetId="9" r:id="rId9"/>
-    <sheet name="fc" sheetId="7" r:id="rId10"/>
-    <sheet name="min_genration" sheetId="6" r:id="rId11"/>
-    <sheet name="max_genration" sheetId="5" r:id="rId12"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId13"/>
+    <sheet name="attributes" sheetId="2" r:id="rId4"/>
+    <sheet name="rules" sheetId="13" r:id="rId5"/>
+    <sheet name="connectivity_matrix" sheetId="12" r:id="rId6"/>
+    <sheet name="fixed_power_flow" sheetId="9" r:id="rId7"/>
+    <sheet name="fc" sheetId="7" r:id="rId8"/>
+    <sheet name="min_genration" sheetId="6" r:id="rId9"/>
+    <sheet name="max_genration" sheetId="5" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId11"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="73">
   <si>
     <t>Name</t>
   </si>
@@ -227,19 +225,34 @@
     <t>a8_a1</t>
   </si>
   <si>
-    <t>mrf</t>
-  </si>
-  <si>
-    <t>Member</t>
-  </si>
-  <si>
-    <t>Node</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
     <t>Text</t>
+  </si>
+  <si>
+    <t>Maximum  production of genration node</t>
+  </si>
+  <si>
+    <t>Minimum  production of genration node</t>
+  </si>
+  <si>
+    <t>fixed_consumers</t>
+  </si>
+  <si>
+    <t>fixed_generators</t>
+  </si>
+  <si>
+    <t>fixed_genration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fixed  consummation   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>fixed_consummation</t>
   </si>
 </sst>
 </file>
@@ -609,211 +622,6 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B1" location="nodes!A4" tooltip="Browse to a2" display="a2"/>
-    <hyperlink ref="B3" location="attributes!A6" tooltip="Browse to fc" display="fc"/>
-    <hyperlink ref="D1" location="nodes!A6" tooltip="Browse to a4" display="a4"/>
-    <hyperlink ref="D3" location="attributes!A6" tooltip="Browse to fc" display="fc"/>
-    <hyperlink ref="F3" location="attributes!A6" tooltip="Browse to fc" display="fc"/>
-    <hyperlink ref="F1" location="nodes!A10" tooltip="Browse to a8" display="a8"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B1" location="nodes!A3" tooltip="Browse to a1" display="a1"/>
-    <hyperlink ref="B3" location="attributes!A7" tooltip="Browse to min_genration" display="min_genration"/>
-    <hyperlink ref="D1" location="nodes!A7" tooltip="Browse to a5" display="a5"/>
-    <hyperlink ref="D3" location="attributes!A7" tooltip="Browse to min_genration" display="min_genration"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -902,7 +710,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -916,26 +724,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -958,16 +767,19 @@
         <v>12</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -978,7 +790,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1000,11 +812,11 @@
       <c r="G3" s="1">
         <v>0</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1015,16 +827,13 @@
         <v>4892819</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="H4" s="1">
         <v>10</v>
       </c>
-      <c r="I4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -1038,7 +847,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1049,16 +858,13 @@
         <v>4817014</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="H6" s="1">
         <v>80</v>
       </c>
-      <c r="I6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1069,22 +875,21 @@
         <v>4747957</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="1">
+        <v>71</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="J7">
         <v>100</v>
       </c>
-      <c r="G7" s="1">
-        <v>100</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1098,7 +903,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -1115,7 +920,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1126,13 +931,10 @@
         <v>4772510</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="H10" s="1">
         <v>30</v>
-      </c>
-      <c r="I10" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1140,8 +942,6 @@
     <hyperlink ref="H1" location="attributes!A6" tooltip="Browse to fc" display="fc"/>
     <hyperlink ref="I1" location="attributes!A2" tooltip="Browse to power_consumption" display="power_consumption"/>
     <hyperlink ref="H4" location="fc!B3" tooltip="Browse to 10" display="10"/>
-    <hyperlink ref="F7" location="max_genration!D3" tooltip="Browse to 100" display="100"/>
-    <hyperlink ref="G7" location="min_genration!D3" tooltip="Browse to 100" display="100"/>
     <hyperlink ref="E1" location="attributes!A3" tooltip="Browse to power_generation" display="power_generation"/>
     <hyperlink ref="H6" location="fc!D3" tooltip="Browse to 80" display="80"/>
     <hyperlink ref="F3" location="max_genration!B3" tooltip="Browse to 900" display="900"/>
@@ -1557,34 +1357,129 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1594,186 +1489,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" location="nodes!A4" tooltip="Browse to a2" display="a2"/>
-    <hyperlink ref="C3" location="nodes!A6" tooltip="Browse to a4" display="a4"/>
-    <hyperlink ref="C4" location="nodes!A10" tooltip="Browse to a8" display="a8"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1788,7 +1508,7 @@
         <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -1799,7 +1519,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -1841,25 +1561,25 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I2" t="s">
         <v>23</v>
@@ -1873,25 +1593,25 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
         <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1899,28 +1619,28 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
         <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H4" t="s">
         <v>23</v>
       </c>
       <c r="I4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1928,28 +1648,28 @@
         <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
         <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F5" t="s">
         <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1957,28 +1677,28 @@
         <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E6" t="s">
         <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G6" t="s">
         <v>23</v>
       </c>
       <c r="H6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1986,22 +1706,22 @@
         <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F7" t="s">
         <v>23</v>
       </c>
       <c r="G7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H7" t="s">
         <v>23</v>
@@ -2015,28 +1735,28 @@
         <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D8" t="s">
         <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G8" t="s">
         <v>23</v>
       </c>
       <c r="H8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2047,25 +1767,25 @@
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G9" t="s">
         <v>23</v>
       </c>
       <c r="H9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2091,7 +1811,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -2179,4 +1899,209 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" location="nodes!A4" tooltip="Browse to a2" display="a2"/>
+    <hyperlink ref="B3" location="attributes!A6" tooltip="Browse to fc" display="fc"/>
+    <hyperlink ref="D1" location="nodes!A6" tooltip="Browse to a4" display="a4"/>
+    <hyperlink ref="D3" location="attributes!A6" tooltip="Browse to fc" display="fc"/>
+    <hyperlink ref="F3" location="attributes!A6" tooltip="Browse to fc" display="fc"/>
+    <hyperlink ref="F1" location="nodes!A10" tooltip="Browse to a8" display="a8"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" location="nodes!A3" tooltip="Browse to a1" display="a1"/>
+    <hyperlink ref="B3" location="attributes!A7" tooltip="Browse to min_genration" display="min_genration"/>
+    <hyperlink ref="D1" location="nodes!A7" tooltip="Browse to a5" display="a5"/>
+    <hyperlink ref="D3" location="attributes!A7" tooltip="Browse to min_genration" display="min_genration"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>